<commit_message>
fix: further translation fixes
</commit_message>
<xml_diff>
--- a/docassemble/ukraine/data/sources/interview_en.xlsx
+++ b/docassemble/ukraine/data/sources/interview_en.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/felixvemmer/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80124B29-0624-3340-B15C-A20B90E459E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF3250C6-6767-C945-83FD-6C6F9B47178B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1114" uniqueCount="447">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1114" uniqueCount="448">
   <si>
     <t>interview</t>
   </si>
@@ -406,7 +406,7 @@
     <t>Größe in cm</t>
   </si>
   <si>
-    <t/>
+    <t>Height in cm</t>
   </si>
   <si>
     <t>4481872be58c4d95aec1336303b73159</t>
@@ -862,39 +862,6 @@
       </rPr>
       <t xml:space="preserve">. Familienmitglied
 </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Please complete the information about your </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>${ i + 1 }</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>. Family member</t>
     </r>
   </si>
   <si>
@@ -2009,9 +1976,6 @@
     <t>Größe</t>
   </si>
   <si>
-    <t>Height in cm</t>
-  </si>
-  <si>
     <t>eaf88f9c5a548686fa745ff9dc445775</t>
   </si>
   <si>
@@ -2030,6 +1994,38 @@
   <si>
     <t xml:space="preserve">Please watch the video below and follow the instructions to find the **right address** to send your application
 </t>
+  </si>
+  <si>
+    <t>registered with mother</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Please complete the information about your </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>${ i + 1 }</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>. family member</t>
+    </r>
+  </si>
+  <si>
+    <t>restricted to</t>
   </si>
 </sst>
 </file>
@@ -2441,8 +2437,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H159"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="H43" sqref="H43"/>
+    <sheetView tabSelected="1" topLeftCell="A154" workbookViewId="0">
+      <selection activeCell="H133" sqref="H133"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3542,7 +3538,7 @@
         <v>115</v>
       </c>
       <c r="H42" s="4" t="s">
-        <v>440</v>
+        <v>116</v>
       </c>
     </row>
     <row r="43" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -4192,7 +4188,7 @@
         <v>187</v>
       </c>
       <c r="H67" s="4" t="s">
-        <v>116</v>
+        <v>445</v>
       </c>
     </row>
     <row r="68" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -4842,7 +4838,7 @@
         <v>255</v>
       </c>
       <c r="H92" s="4" t="s">
-        <v>256</v>
+        <v>446</v>
       </c>
     </row>
     <row r="93" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -4856,19 +4852,19 @@
         <v>2</v>
       </c>
       <c r="D93" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="E93" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F93" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G93" s="3" t="s">
         <v>257</v>
       </c>
-      <c r="E93" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F93" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G93" s="3" t="s">
-        <v>258</v>
-      </c>
       <c r="H93" s="4" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="94" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -4882,19 +4878,19 @@
         <v>3</v>
       </c>
       <c r="D94" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="E94" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F94" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G94" s="3" t="s">
         <v>259</v>
       </c>
-      <c r="E94" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F94" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G94" s="3" t="s">
+      <c r="H94" s="4" t="s">
         <v>260</v>
-      </c>
-      <c r="H94" s="4" t="s">
-        <v>261</v>
       </c>
     </row>
     <row r="95" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -4908,19 +4904,19 @@
         <v>4</v>
       </c>
       <c r="D95" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="E95" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F95" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G95" s="3" t="s">
         <v>262</v>
       </c>
-      <c r="E95" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F95" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G95" s="3" t="s">
+      <c r="H95" s="4" t="s">
         <v>263</v>
-      </c>
-      <c r="H95" s="4" t="s">
-        <v>264</v>
       </c>
     </row>
     <row r="96" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -4934,19 +4930,19 @@
         <v>5</v>
       </c>
       <c r="D96" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="E96" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F96" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G96" s="3" t="s">
         <v>265</v>
       </c>
-      <c r="E96" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F96" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G96" s="3" t="s">
+      <c r="H96" s="4" t="s">
         <v>266</v>
-      </c>
-      <c r="H96" s="4" t="s">
-        <v>267</v>
       </c>
     </row>
     <row r="97" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -4960,19 +4956,19 @@
         <v>6</v>
       </c>
       <c r="D97" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="E97" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F97" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G97" s="3" t="s">
         <v>268</v>
       </c>
-      <c r="E97" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F97" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G97" s="3" t="s">
+      <c r="H97" s="4" t="s">
         <v>269</v>
-      </c>
-      <c r="H97" s="4" t="s">
-        <v>270</v>
       </c>
     </row>
     <row r="98" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -4986,19 +4982,19 @@
         <v>7</v>
       </c>
       <c r="D98" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="E98" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F98" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G98" s="3" t="s">
         <v>271</v>
       </c>
-      <c r="E98" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F98" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G98" s="3" t="s">
+      <c r="H98" s="4" t="s">
         <v>272</v>
-      </c>
-      <c r="H98" s="4" t="s">
-        <v>273</v>
       </c>
     </row>
     <row r="99" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -5012,19 +5008,19 @@
         <v>8</v>
       </c>
       <c r="D99" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="E99" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F99" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G99" s="3" t="s">
         <v>274</v>
       </c>
-      <c r="E99" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F99" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G99" s="3" t="s">
+      <c r="H99" s="4" t="s">
         <v>275</v>
-      </c>
-      <c r="H99" s="4" t="s">
-        <v>276</v>
       </c>
     </row>
     <row r="100" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -5038,19 +5034,19 @@
         <v>9</v>
       </c>
       <c r="D100" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="E100" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F100" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G100" s="3" t="s">
         <v>277</v>
       </c>
-      <c r="E100" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F100" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G100" s="3" t="s">
+      <c r="H100" s="4" t="s">
         <v>278</v>
-      </c>
-      <c r="H100" s="4" t="s">
-        <v>279</v>
       </c>
     </row>
     <row r="101" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -5064,19 +5060,19 @@
         <v>10</v>
       </c>
       <c r="D101" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="E101" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F101" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G101" s="3" t="s">
         <v>280</v>
       </c>
-      <c r="E101" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F101" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G101" s="3" t="s">
+      <c r="H101" s="4" t="s">
         <v>281</v>
-      </c>
-      <c r="H101" s="4" t="s">
-        <v>282</v>
       </c>
     </row>
     <row r="102" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -5090,19 +5086,19 @@
         <v>11</v>
       </c>
       <c r="D102" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="E102" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F102" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G102" s="3" t="s">
         <v>283</v>
       </c>
-      <c r="E102" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F102" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G102" s="3" t="s">
+      <c r="H102" s="4" t="s">
         <v>284</v>
-      </c>
-      <c r="H102" s="4" t="s">
-        <v>285</v>
       </c>
     </row>
     <row r="103" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -5116,19 +5112,19 @@
         <v>12</v>
       </c>
       <c r="D103" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="E103" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F103" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G103" s="3" t="s">
         <v>286</v>
       </c>
-      <c r="E103" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F103" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G103" s="3" t="s">
+      <c r="H103" s="4" t="s">
         <v>287</v>
-      </c>
-      <c r="H103" s="4" t="s">
-        <v>288</v>
       </c>
     </row>
     <row r="104" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -5142,19 +5138,19 @@
         <v>13</v>
       </c>
       <c r="D104" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="E104" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F104" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G104" s="3" t="s">
         <v>289</v>
       </c>
-      <c r="E104" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F104" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G104" s="3" t="s">
+      <c r="H104" s="4" t="s">
         <v>290</v>
-      </c>
-      <c r="H104" s="4" t="s">
-        <v>291</v>
       </c>
     </row>
     <row r="105" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -5168,19 +5164,19 @@
         <v>14</v>
       </c>
       <c r="D105" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="E105" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F105" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G105" s="3" t="s">
         <v>292</v>
       </c>
-      <c r="E105" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F105" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G105" s="3" t="s">
+      <c r="H105" s="4" t="s">
         <v>293</v>
-      </c>
-      <c r="H105" s="4" t="s">
-        <v>294</v>
       </c>
     </row>
     <row r="106" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -5194,19 +5190,19 @@
         <v>15</v>
       </c>
       <c r="D106" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="E106" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F106" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G106" s="3" t="s">
         <v>295</v>
       </c>
-      <c r="E106" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F106" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G106" s="3" t="s">
+      <c r="H106" s="4" t="s">
         <v>296</v>
-      </c>
-      <c r="H106" s="4" t="s">
-        <v>297</v>
       </c>
     </row>
     <row r="107" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -5220,19 +5216,19 @@
         <v>16</v>
       </c>
       <c r="D107" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="E107" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F107" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G107" s="3" t="s">
         <v>298</v>
       </c>
-      <c r="E107" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F107" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G107" s="3" t="s">
+      <c r="H107" s="4" t="s">
         <v>299</v>
-      </c>
-      <c r="H107" s="4" t="s">
-        <v>300</v>
       </c>
     </row>
     <row r="108" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -5246,7 +5242,7 @@
         <v>17</v>
       </c>
       <c r="D108" s="2" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="E108" s="2" t="s">
         <v>11</v>
@@ -5255,10 +5251,10 @@
         <v>12</v>
       </c>
       <c r="G108" s="3" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="H108" s="4" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="109" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -5266,25 +5262,25 @@
         <v>8</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C109" s="2">
         <v>0</v>
       </c>
       <c r="D109" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="E109" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F109" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G109" s="3" t="s">
         <v>303</v>
       </c>
-      <c r="E109" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F109" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G109" s="3" t="s">
-        <v>304</v>
-      </c>
       <c r="H109" s="4" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="110" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -5292,25 +5288,25 @@
         <v>8</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C110" s="2">
         <v>1</v>
       </c>
       <c r="D110" s="2" t="s">
+        <v>304</v>
+      </c>
+      <c r="E110" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F110" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G110" s="3" t="s">
         <v>305</v>
       </c>
-      <c r="E110" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F110" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G110" s="3" t="s">
+      <c r="H110" s="4" t="s">
         <v>306</v>
-      </c>
-      <c r="H110" s="4" t="s">
-        <v>307</v>
       </c>
     </row>
     <row r="111" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -5318,25 +5314,25 @@
         <v>8</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C111" s="2">
         <v>0</v>
       </c>
       <c r="D111" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="E111" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F111" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G111" s="3" t="s">
         <v>309</v>
       </c>
-      <c r="E111" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F111" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G111" s="3" t="s">
-        <v>310</v>
-      </c>
       <c r="H111" s="4" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="112" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -5344,25 +5340,25 @@
         <v>8</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C112" s="2">
         <v>1</v>
       </c>
       <c r="D112" s="2" t="s">
+        <v>310</v>
+      </c>
+      <c r="E112" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F112" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G112" s="3" t="s">
         <v>311</v>
       </c>
-      <c r="E112" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F112" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G112" s="3" t="s">
+      <c r="H112" s="4" t="s">
         <v>312</v>
-      </c>
-      <c r="H112" s="4" t="s">
-        <v>313</v>
       </c>
     </row>
     <row r="113" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -5370,25 +5366,25 @@
         <v>8</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C113" s="2">
         <v>2</v>
       </c>
       <c r="D113" s="2" t="s">
+        <v>313</v>
+      </c>
+      <c r="E113" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F113" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G113" s="3" t="s">
         <v>314</v>
       </c>
-      <c r="E113" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F113" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G113" s="3" t="s">
+      <c r="H113" s="4" t="s">
         <v>315</v>
-      </c>
-      <c r="H113" s="4" t="s">
-        <v>316</v>
       </c>
     </row>
     <row r="114" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -5396,25 +5392,25 @@
         <v>8</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C114" s="2">
         <v>3</v>
       </c>
       <c r="D114" s="2" t="s">
+        <v>316</v>
+      </c>
+      <c r="E114" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F114" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G114" s="3" t="s">
         <v>317</v>
       </c>
-      <c r="E114" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F114" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G114" s="3" t="s">
+      <c r="H114" s="4" t="s">
         <v>318</v>
-      </c>
-      <c r="H114" s="4" t="s">
-        <v>319</v>
       </c>
     </row>
     <row r="115" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -5422,25 +5418,25 @@
         <v>8</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C115" s="2">
         <v>4</v>
       </c>
       <c r="D115" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="E115" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F115" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G115" s="3" t="s">
         <v>320</v>
       </c>
-      <c r="E115" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F115" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G115" s="3" t="s">
+      <c r="H115" s="4" t="s">
         <v>321</v>
-      </c>
-      <c r="H115" s="4" t="s">
-        <v>322</v>
       </c>
     </row>
     <row r="116" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -5448,25 +5444,25 @@
         <v>8</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C116" s="2">
         <v>5</v>
       </c>
       <c r="D116" s="2" t="s">
+        <v>322</v>
+      </c>
+      <c r="E116" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F116" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G116" s="3" t="s">
         <v>323</v>
       </c>
-      <c r="E116" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F116" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G116" s="3" t="s">
+      <c r="H116" s="4" t="s">
         <v>324</v>
-      </c>
-      <c r="H116" s="4" t="s">
-        <v>325</v>
       </c>
     </row>
     <row r="117" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -5474,25 +5470,25 @@
         <v>8</v>
       </c>
       <c r="B117" s="2" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C117" s="2">
         <v>6</v>
       </c>
       <c r="D117" s="2" t="s">
+        <v>325</v>
+      </c>
+      <c r="E117" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F117" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G117" s="3" t="s">
         <v>326</v>
       </c>
-      <c r="E117" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F117" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G117" s="3" t="s">
+      <c r="H117" s="4" t="s">
         <v>327</v>
-      </c>
-      <c r="H117" s="4" t="s">
-        <v>328</v>
       </c>
     </row>
     <row r="118" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -5500,25 +5496,25 @@
         <v>8</v>
       </c>
       <c r="B118" s="2" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C118" s="2">
         <v>7</v>
       </c>
       <c r="D118" s="2" t="s">
+        <v>328</v>
+      </c>
+      <c r="E118" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F118" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G118" s="3" t="s">
         <v>329</v>
       </c>
-      <c r="E118" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F118" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G118" s="3" t="s">
+      <c r="H118" s="4" t="s">
         <v>330</v>
-      </c>
-      <c r="H118" s="4" t="s">
-        <v>331</v>
       </c>
     </row>
     <row r="119" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -5526,25 +5522,25 @@
         <v>8</v>
       </c>
       <c r="B119" s="2" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C119" s="2">
         <v>8</v>
       </c>
       <c r="D119" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="E119" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F119" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G119" s="3" t="s">
         <v>332</v>
       </c>
-      <c r="E119" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F119" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G119" s="3" t="s">
-        <v>333</v>
-      </c>
       <c r="H119" s="4" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="120" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -5552,25 +5548,25 @@
         <v>8</v>
       </c>
       <c r="B120" s="2" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C120" s="2">
         <v>9</v>
       </c>
       <c r="D120" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="E120" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F120" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G120" s="3" t="s">
         <v>334</v>
       </c>
-      <c r="E120" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F120" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G120" s="3" t="s">
+      <c r="H120" s="4" t="s">
         <v>335</v>
-      </c>
-      <c r="H120" s="4" t="s">
-        <v>336</v>
       </c>
     </row>
     <row r="121" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -5578,25 +5574,25 @@
         <v>8</v>
       </c>
       <c r="B121" s="2" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C121" s="2">
         <v>10</v>
       </c>
       <c r="D121" s="2" t="s">
+        <v>336</v>
+      </c>
+      <c r="E121" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F121" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G121" s="3" t="s">
         <v>337</v>
       </c>
-      <c r="E121" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F121" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G121" s="3" t="s">
+      <c r="H121" s="4" t="s">
         <v>338</v>
-      </c>
-      <c r="H121" s="4" t="s">
-        <v>339</v>
       </c>
     </row>
     <row r="122" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -5604,25 +5600,25 @@
         <v>8</v>
       </c>
       <c r="B122" s="2" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C122" s="2">
         <v>11</v>
       </c>
       <c r="D122" s="2" t="s">
+        <v>339</v>
+      </c>
+      <c r="E122" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F122" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G122" s="3" t="s">
         <v>340</v>
       </c>
-      <c r="E122" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F122" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G122" s="3" t="s">
+      <c r="H122" s="4" t="s">
         <v>341</v>
-      </c>
-      <c r="H122" s="4" t="s">
-        <v>342</v>
       </c>
     </row>
     <row r="123" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -5630,25 +5626,25 @@
         <v>8</v>
       </c>
       <c r="B123" s="2" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C123" s="2">
         <v>12</v>
       </c>
       <c r="D123" s="2" t="s">
+        <v>342</v>
+      </c>
+      <c r="E123" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F123" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G123" s="3" t="s">
         <v>343</v>
       </c>
-      <c r="E123" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F123" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G123" s="3" t="s">
+      <c r="H123" s="4" t="s">
         <v>344</v>
-      </c>
-      <c r="H123" s="4" t="s">
-        <v>345</v>
       </c>
     </row>
     <row r="124" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -5656,25 +5652,25 @@
         <v>8</v>
       </c>
       <c r="B124" s="2" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C124" s="2">
         <v>13</v>
       </c>
       <c r="D124" s="2" t="s">
+        <v>345</v>
+      </c>
+      <c r="E124" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F124" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G124" s="3" t="s">
         <v>346</v>
       </c>
-      <c r="E124" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F124" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G124" s="3" t="s">
-        <v>347</v>
-      </c>
       <c r="H124" s="4" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="125" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -5682,25 +5678,25 @@
         <v>8</v>
       </c>
       <c r="B125" s="2" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C125" s="2">
         <v>14</v>
       </c>
       <c r="D125" s="2" t="s">
+        <v>347</v>
+      </c>
+      <c r="E125" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F125" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G125" s="3" t="s">
         <v>348</v>
       </c>
-      <c r="E125" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F125" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G125" s="3" t="s">
+      <c r="H125" s="4" t="s">
         <v>349</v>
-      </c>
-      <c r="H125" s="4" t="s">
-        <v>350</v>
       </c>
     </row>
     <row r="126" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -5708,25 +5704,25 @@
         <v>8</v>
       </c>
       <c r="B126" s="2" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C126" s="2">
         <v>15</v>
       </c>
       <c r="D126" s="2" t="s">
+        <v>350</v>
+      </c>
+      <c r="E126" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F126" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G126" s="3" t="s">
         <v>351</v>
       </c>
-      <c r="E126" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F126" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G126" s="3" t="s">
-        <v>352</v>
-      </c>
       <c r="H126" s="4" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="127" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -5734,25 +5730,25 @@
         <v>8</v>
       </c>
       <c r="B127" s="2" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C127" s="2">
         <v>16</v>
       </c>
       <c r="D127" s="2" t="s">
+        <v>352</v>
+      </c>
+      <c r="E127" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F127" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G127" s="3" t="s">
         <v>353</v>
       </c>
-      <c r="E127" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F127" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G127" s="3" t="s">
+      <c r="H127" s="4" t="s">
         <v>354</v>
-      </c>
-      <c r="H127" s="4" t="s">
-        <v>355</v>
       </c>
     </row>
     <row r="128" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -5760,25 +5756,25 @@
         <v>8</v>
       </c>
       <c r="B128" s="2" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C128" s="2">
         <v>17</v>
       </c>
       <c r="D128" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="E128" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F128" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G128" s="3" t="s">
         <v>356</v>
       </c>
-      <c r="E128" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F128" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G128" s="3" t="s">
+      <c r="H128" s="4" t="s">
         <v>357</v>
-      </c>
-      <c r="H128" s="4" t="s">
-        <v>358</v>
       </c>
     </row>
     <row r="129" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -5786,25 +5782,25 @@
         <v>8</v>
       </c>
       <c r="B129" s="2" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C129" s="2">
         <v>18</v>
       </c>
       <c r="D129" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="E129" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F129" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G129" s="3" t="s">
         <v>359</v>
       </c>
-      <c r="E129" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F129" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G129" s="3" t="s">
+      <c r="H129" s="4" t="s">
         <v>360</v>
-      </c>
-      <c r="H129" s="4" t="s">
-        <v>361</v>
       </c>
     </row>
     <row r="130" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -5812,25 +5808,25 @@
         <v>8</v>
       </c>
       <c r="B130" s="2" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C130" s="2">
         <v>19</v>
       </c>
       <c r="D130" s="2" t="s">
+        <v>361</v>
+      </c>
+      <c r="E130" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F130" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G130" s="3" t="s">
         <v>362</v>
       </c>
-      <c r="E130" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F130" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G130" s="3" t="s">
+      <c r="H130" s="4" t="s">
         <v>363</v>
-      </c>
-      <c r="H130" s="4" t="s">
-        <v>364</v>
       </c>
     </row>
     <row r="131" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -5838,25 +5834,25 @@
         <v>8</v>
       </c>
       <c r="B131" s="2" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C131" s="2">
         <v>20</v>
       </c>
       <c r="D131" s="2" t="s">
+        <v>364</v>
+      </c>
+      <c r="E131" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F131" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G131" s="3" t="s">
         <v>365</v>
       </c>
-      <c r="E131" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F131" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G131" s="3" t="s">
+      <c r="H131" s="4" t="s">
         <v>366</v>
-      </c>
-      <c r="H131" s="4" t="s">
-        <v>367</v>
       </c>
     </row>
     <row r="132" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -5864,25 +5860,25 @@
         <v>8</v>
       </c>
       <c r="B132" s="2" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C132" s="2">
         <v>21</v>
       </c>
       <c r="D132" s="2" t="s">
+        <v>367</v>
+      </c>
+      <c r="E132" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F132" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G132" s="3" t="s">
         <v>368</v>
       </c>
-      <c r="E132" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F132" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G132" s="3" t="s">
-        <v>369</v>
-      </c>
       <c r="H132" s="4" t="s">
-        <v>369</v>
+        <v>447</v>
       </c>
     </row>
     <row r="133" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -5890,25 +5886,25 @@
         <v>8</v>
       </c>
       <c r="B133" s="2" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C133" s="2">
         <v>22</v>
       </c>
       <c r="D133" s="2" t="s">
+        <v>369</v>
+      </c>
+      <c r="E133" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F133" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G133" s="3" t="s">
         <v>370</v>
       </c>
-      <c r="E133" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F133" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G133" s="3" t="s">
+      <c r="H133" s="4" t="s">
         <v>371</v>
-      </c>
-      <c r="H133" s="4" t="s">
-        <v>372</v>
       </c>
     </row>
     <row r="134" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -5916,25 +5912,25 @@
         <v>8</v>
       </c>
       <c r="B134" s="2" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="C134" s="2">
         <v>0</v>
       </c>
       <c r="D134" s="2" t="s">
+        <v>373</v>
+      </c>
+      <c r="E134" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F134" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G134" s="3" t="s">
         <v>374</v>
       </c>
-      <c r="E134" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F134" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G134" s="3" t="s">
-        <v>375</v>
-      </c>
       <c r="H134" s="4" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="135" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -5942,25 +5938,25 @@
         <v>8</v>
       </c>
       <c r="B135" s="2" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="C135" s="2">
         <v>1</v>
       </c>
       <c r="D135" s="2" t="s">
+        <v>375</v>
+      </c>
+      <c r="E135" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F135" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G135" s="3" t="s">
         <v>376</v>
       </c>
-      <c r="E135" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F135" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G135" s="3" t="s">
+      <c r="H135" s="4" t="s">
         <v>377</v>
-      </c>
-      <c r="H135" s="4" t="s">
-        <v>378</v>
       </c>
     </row>
     <row r="136" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -5968,25 +5964,25 @@
         <v>8</v>
       </c>
       <c r="B136" s="2" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="C136" s="2">
         <v>2</v>
       </c>
       <c r="D136" s="2" t="s">
+        <v>378</v>
+      </c>
+      <c r="E136" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F136" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G136" s="3" t="s">
         <v>379</v>
       </c>
-      <c r="E136" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F136" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G136" s="3" t="s">
+      <c r="H136" s="4" t="s">
         <v>380</v>
-      </c>
-      <c r="H136" s="4" t="s">
-        <v>381</v>
       </c>
     </row>
     <row r="137" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -5994,25 +5990,25 @@
         <v>8</v>
       </c>
       <c r="B137" s="2" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="C137" s="2">
         <v>3</v>
       </c>
       <c r="D137" s="2" t="s">
+        <v>381</v>
+      </c>
+      <c r="E137" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F137" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G137" s="3" t="s">
         <v>382</v>
       </c>
-      <c r="E137" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F137" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G137" s="3" t="s">
+      <c r="H137" s="4" t="s">
         <v>383</v>
-      </c>
-      <c r="H137" s="4" t="s">
-        <v>384</v>
       </c>
     </row>
     <row r="138" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -6020,25 +6016,25 @@
         <v>8</v>
       </c>
       <c r="B138" s="2" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="C138" s="2">
         <v>4</v>
       </c>
       <c r="D138" s="2" t="s">
+        <v>384</v>
+      </c>
+      <c r="E138" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F138" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G138" s="3" t="s">
         <v>385</v>
       </c>
-      <c r="E138" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F138" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G138" s="3" t="s">
-        <v>386</v>
-      </c>
       <c r="H138" s="4" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="139" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -6046,25 +6042,25 @@
         <v>8</v>
       </c>
       <c r="B139" s="2" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="C139" s="2">
         <v>5</v>
       </c>
       <c r="D139" s="2" t="s">
+        <v>386</v>
+      </c>
+      <c r="E139" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F139" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G139" s="3" t="s">
         <v>387</v>
       </c>
-      <c r="E139" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F139" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G139" s="3" t="s">
+      <c r="H139" s="4" t="s">
         <v>388</v>
-      </c>
-      <c r="H139" s="4" t="s">
-        <v>389</v>
       </c>
     </row>
     <row r="140" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -6072,25 +6068,25 @@
         <v>8</v>
       </c>
       <c r="B140" s="2" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="C140" s="2">
         <v>6</v>
       </c>
       <c r="D140" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="E140" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F140" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G140" s="3" t="s">
         <v>390</v>
       </c>
-      <c r="E140" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F140" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G140" s="3" t="s">
+      <c r="H140" s="4" t="s">
         <v>391</v>
-      </c>
-      <c r="H140" s="4" t="s">
-        <v>392</v>
       </c>
     </row>
     <row r="141" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -6098,25 +6094,25 @@
         <v>8</v>
       </c>
       <c r="B141" s="2" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="C141" s="2">
         <v>7</v>
       </c>
       <c r="D141" s="2" t="s">
+        <v>392</v>
+      </c>
+      <c r="E141" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F141" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G141" s="3" t="s">
         <v>393</v>
       </c>
-      <c r="E141" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F141" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G141" s="3" t="s">
-        <v>394</v>
-      </c>
       <c r="H141" s="4" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="142" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -6124,25 +6120,25 @@
         <v>8</v>
       </c>
       <c r="B142" s="2" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="C142" s="2">
         <v>8</v>
       </c>
       <c r="D142" s="2" t="s">
+        <v>394</v>
+      </c>
+      <c r="E142" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F142" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G142" s="3" t="s">
         <v>395</v>
       </c>
-      <c r="E142" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F142" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G142" s="3" t="s">
+      <c r="H142" s="4" t="s">
         <v>396</v>
-      </c>
-      <c r="H142" s="4" t="s">
-        <v>397</v>
       </c>
     </row>
     <row r="143" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -6150,25 +6146,25 @@
         <v>8</v>
       </c>
       <c r="B143" s="2" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="C143" s="2">
         <v>9</v>
       </c>
       <c r="D143" s="2" t="s">
+        <v>397</v>
+      </c>
+      <c r="E143" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F143" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G143" s="3" t="s">
         <v>398</v>
       </c>
-      <c r="E143" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F143" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G143" s="3" t="s">
-        <v>399</v>
-      </c>
       <c r="H143" s="4" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="144" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -6176,25 +6172,25 @@
         <v>8</v>
       </c>
       <c r="B144" s="2" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="C144" s="2">
         <v>10</v>
       </c>
       <c r="D144" s="2" t="s">
+        <v>399</v>
+      </c>
+      <c r="E144" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F144" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G144" s="3" t="s">
         <v>400</v>
       </c>
-      <c r="E144" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F144" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G144" s="3" t="s">
+      <c r="H144" s="4" t="s">
         <v>401</v>
-      </c>
-      <c r="H144" s="4" t="s">
-        <v>402</v>
       </c>
     </row>
     <row r="145" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -6202,25 +6198,25 @@
         <v>8</v>
       </c>
       <c r="B145" s="2" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="C145" s="2">
         <v>11</v>
       </c>
       <c r="D145" s="2" t="s">
+        <v>402</v>
+      </c>
+      <c r="E145" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F145" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G145" s="3" t="s">
         <v>403</v>
       </c>
-      <c r="E145" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F145" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G145" s="3" t="s">
+      <c r="H145" s="4" t="s">
         <v>404</v>
-      </c>
-      <c r="H145" s="4" t="s">
-        <v>405</v>
       </c>
     </row>
     <row r="146" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -6228,25 +6224,25 @@
         <v>8</v>
       </c>
       <c r="B146" s="2" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="C146" s="2">
         <v>0</v>
       </c>
       <c r="D146" s="2" t="s">
+        <v>406</v>
+      </c>
+      <c r="E146" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F146" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G146" s="3" t="s">
         <v>407</v>
       </c>
-      <c r="E146" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F146" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G146" s="3" t="s">
-        <v>408</v>
-      </c>
       <c r="H146" s="4" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="147" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -6254,25 +6250,25 @@
         <v>8</v>
       </c>
       <c r="B147" s="2" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="C147" s="2">
         <v>1</v>
       </c>
       <c r="D147" s="2" t="s">
+        <v>408</v>
+      </c>
+      <c r="E147" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F147" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G147" s="3" t="s">
         <v>409</v>
       </c>
-      <c r="E147" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F147" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G147" s="3" t="s">
+      <c r="H147" s="4" t="s">
         <v>410</v>
-      </c>
-      <c r="H147" s="4" t="s">
-        <v>411</v>
       </c>
     </row>
     <row r="148" spans="1:8" ht="105" customHeight="1" x14ac:dyDescent="0.2">
@@ -6280,25 +6276,25 @@
         <v>8</v>
       </c>
       <c r="B148" s="2" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="C148" s="2">
         <v>2</v>
       </c>
       <c r="D148" s="2" t="s">
+        <v>411</v>
+      </c>
+      <c r="E148" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F148" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G148" s="3" t="s">
         <v>412</v>
       </c>
-      <c r="E148" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F148" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G148" s="3" t="s">
+      <c r="H148" s="4" t="s">
         <v>413</v>
-      </c>
-      <c r="H148" s="4" t="s">
-        <v>414</v>
       </c>
     </row>
     <row r="149" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -6306,25 +6302,25 @@
         <v>8</v>
       </c>
       <c r="B149" s="2" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="C149" s="2">
         <v>3</v>
       </c>
       <c r="D149" s="2" t="s">
+        <v>414</v>
+      </c>
+      <c r="E149" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F149" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G149" s="5" t="s">
         <v>415</v>
       </c>
-      <c r="E149" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F149" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G149" s="5" t="s">
-        <v>416</v>
-      </c>
       <c r="H149" s="6" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="150" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -6332,25 +6328,25 @@
         <v>8</v>
       </c>
       <c r="B150" s="2" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="C150" s="2">
         <v>4</v>
       </c>
       <c r="D150" s="2" t="s">
+        <v>416</v>
+      </c>
+      <c r="E150" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F150" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G150" s="3" t="s">
         <v>417</v>
       </c>
-      <c r="E150" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F150" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G150" s="3" t="s">
+      <c r="H150" s="4" t="s">
         <v>418</v>
-      </c>
-      <c r="H150" s="4" t="s">
-        <v>419</v>
       </c>
     </row>
     <row r="151" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -6358,126 +6354,126 @@
         <v>8</v>
       </c>
       <c r="B151" s="2" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="C151" s="2">
         <v>5</v>
       </c>
       <c r="D151" s="2" t="s">
+        <v>419</v>
+      </c>
+      <c r="E151" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F151" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G151" s="3" t="s">
         <v>420</v>
       </c>
-      <c r="E151" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F151" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G151" s="3" t="s">
+      <c r="H151" s="4" t="s">
         <v>421</v>
-      </c>
-      <c r="H151" s="4" t="s">
-        <v>422</v>
       </c>
     </row>
     <row r="152" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A152" s="2" t="s">
+        <v>422</v>
+      </c>
+      <c r="B152" s="2" t="s">
         <v>423</v>
-      </c>
-      <c r="B152" s="2" t="s">
-        <v>424</v>
       </c>
       <c r="C152" s="2">
         <v>0</v>
       </c>
       <c r="D152" s="2" t="s">
+        <v>424</v>
+      </c>
+      <c r="E152" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F152" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G152" s="3" t="s">
         <v>425</v>
       </c>
-      <c r="E152" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F152" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G152" s="3" t="s">
-        <v>426</v>
-      </c>
       <c r="H152" s="4" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="153" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A153" s="2" t="s">
+        <v>422</v>
+      </c>
+      <c r="B153" s="2" t="s">
         <v>423</v>
-      </c>
-      <c r="B153" s="2" t="s">
-        <v>424</v>
       </c>
       <c r="C153" s="2">
         <v>1</v>
       </c>
       <c r="D153" s="2" t="s">
+        <v>426</v>
+      </c>
+      <c r="E153" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F153" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G153" s="3" t="s">
         <v>427</v>
       </c>
-      <c r="E153" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F153" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G153" s="3" t="s">
+      <c r="H153" s="4" t="s">
         <v>428</v>
-      </c>
-      <c r="H153" s="4" t="s">
-        <v>429</v>
       </c>
     </row>
     <row r="154" spans="1:8" ht="165" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A154" s="2" t="s">
+        <v>422</v>
+      </c>
+      <c r="B154" s="2" t="s">
         <v>423</v>
-      </c>
-      <c r="B154" s="2" t="s">
-        <v>424</v>
       </c>
       <c r="C154" s="2">
         <v>2</v>
       </c>
       <c r="D154" s="2" t="s">
+        <v>429</v>
+      </c>
+      <c r="E154" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F154" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G154" s="3" t="s">
         <v>430</v>
       </c>
-      <c r="E154" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F154" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G154" s="3" t="s">
+      <c r="H154" s="4" t="s">
         <v>431</v>
-      </c>
-      <c r="H154" s="4" t="s">
-        <v>432</v>
       </c>
     </row>
     <row r="155" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A155" s="2" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="B155" s="2" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="C155" s="2">
         <v>0</v>
       </c>
       <c r="D155" s="2" t="s">
+        <v>433</v>
+      </c>
+      <c r="E155" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F155" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G155" s="3" t="s">
         <v>434</v>
-      </c>
-      <c r="E155" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F155" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G155" s="3" t="s">
-        <v>435</v>
       </c>
       <c r="H155" s="4" t="s">
         <v>27</v>
@@ -6485,25 +6481,25 @@
     </row>
     <row r="156" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A156" s="2" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="B156" s="2" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="C156" s="2">
         <v>1</v>
       </c>
       <c r="D156" s="2" t="s">
+        <v>435</v>
+      </c>
+      <c r="E156" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F156" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G156" s="3" t="s">
         <v>436</v>
-      </c>
-      <c r="E156" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F156" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G156" s="3" t="s">
-        <v>437</v>
       </c>
       <c r="H156" s="4" t="s">
         <v>27</v>
@@ -6517,22 +6513,22 @@
         <v>44</v>
       </c>
       <c r="C157" s="2">
-        <v>1026</v>
+        <v>2026</v>
       </c>
       <c r="D157" s="2" t="s">
+        <v>437</v>
+      </c>
+      <c r="E157" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F157" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G157" s="3" t="s">
         <v>438</v>
       </c>
-      <c r="E157" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F157" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G157" s="3" t="s">
-        <v>439</v>
-      </c>
       <c r="H157" s="4" t="s">
-        <v>440</v>
+        <v>116</v>
       </c>
     </row>
     <row r="158" spans="1:8" ht="32" x14ac:dyDescent="0.2">
@@ -6543,22 +6539,22 @@
         <v>171</v>
       </c>
       <c r="C158" s="2">
-        <v>2002</v>
+        <v>3002</v>
       </c>
       <c r="D158" s="2" t="s">
+        <v>439</v>
+      </c>
+      <c r="E158" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F158" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G158" s="3" t="s">
+        <v>440</v>
+      </c>
+      <c r="H158" s="4" t="s">
         <v>441</v>
-      </c>
-      <c r="E158" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F158" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G158" s="3" t="s">
-        <v>442</v>
-      </c>
-      <c r="H158" s="4" t="s">
-        <v>443</v>
       </c>
     </row>
     <row r="159" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -6566,25 +6562,25 @@
         <v>8</v>
       </c>
       <c r="B159" s="2" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C159" s="2">
-        <v>2002</v>
+        <v>3002</v>
       </c>
       <c r="D159" s="2" t="s">
+        <v>442</v>
+      </c>
+      <c r="E159" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F159" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G159" s="3" t="s">
+        <v>443</v>
+      </c>
+      <c r="H159" s="4" t="s">
         <v>444</v>
-      </c>
-      <c r="E159" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F159" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G159" s="3" t="s">
-        <v>445</v>
-      </c>
-      <c r="H159" s="4" t="s">
-        <v>446</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix: fixes en translation
</commit_message>
<xml_diff>
--- a/docassemble/ukraine/data/sources/interview_en.xlsx
+++ b/docassemble/ukraine/data/sources/interview_en.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/felixvemmer/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/felixvemmer/Desktop/tripliq-repo/docassemble-ukraine/docassemble/ukraine/data/sources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF3250C6-6767-C945-83FD-6C6F9B47178B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82915013-054F-1841-95BB-E41FE0894F2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1114" uniqueCount="448">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1114" uniqueCount="449">
   <si>
     <t>interview</t>
   </si>
@@ -2026,6 +2026,9 @@
   </si>
   <si>
     <t>restricted to</t>
+  </si>
+  <si>
+    <t>Escape from war</t>
   </si>
 </sst>
 </file>
@@ -2437,8 +2440,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H159"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A154" workbookViewId="0">
-      <selection activeCell="H133" sqref="H133"/>
+    <sheetView tabSelected="1" topLeftCell="A127" workbookViewId="0">
+      <selection activeCell="H144" sqref="H144"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6164,7 +6167,7 @@
         <v>398</v>
       </c>
       <c r="H143" s="4" t="s">
-        <v>398</v>
+        <v>448</v>
       </c>
     </row>
     <row r="144" spans="1:8" ht="16" x14ac:dyDescent="0.2">

</xml_diff>